<commit_message>
ACU node with the three modules
</commit_message>
<xml_diff>
--- a/Documentation/V_Cycle Process/1.0 Requirements/AEP CAN database.xlsx
+++ b/Documentation/V_Cycle Process/1.0 Requirements/AEP CAN database.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="12240" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="12240" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="118">
   <si>
     <t xml:space="preserve">Message </t>
   </si>
@@ -831,8 +831,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:O27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O20" sqref="O20"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1151,9 +1151,6 @@
       </c>
       <c r="K9" s="3" t="s">
         <v>57</v>
-      </c>
-      <c r="L9" s="3" t="s">
-        <v>58</v>
       </c>
       <c r="N9" s="3" t="s">
         <v>16</v>
@@ -1530,8 +1527,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:O143"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>